<commit_message>
Update Kim's timetable and correct "Note" to "Legend".
</commit_message>
<xml_diff>
--- a/WeeklySchedule.xlsx
+++ b/WeeklySchedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tiết</t>
   </si>
@@ -46,18 +46,30 @@
   </si>
   <si>
     <t>Giờ bắt đầu</t>
+  </si>
+  <si>
+    <t>Legend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -132,6 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,14 +442,14 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="7" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="7" customWidth="1"/>
+    <col min="2" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1" ht="34.5" customHeight="1">
@@ -510,6 +523,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:19">
@@ -518,6 +532,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="3"/>
     </row>
@@ -535,6 +550,7 @@
       <c r="A9" s="6">
         <v>7</v>
       </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="I9" s="9" t="s">
         <v>7</v>
@@ -544,12 +560,14 @@
       <c r="A10" s="6">
         <v>8</v>
       </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6">
         <v>9</v>
       </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -558,6 +576,7 @@
       <c r="A12" s="6">
         <v>10</v>
       </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -566,12 +585,14 @@
       <c r="A13" s="6">
         <v>11</v>
       </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="6">
         <v>12</v>
       </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:19">
@@ -609,7 +630,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="E23" t="s">
+      <c r="E23" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="1"/>
@@ -618,6 +639,9 @@
       </c>
     </row>
     <row r="24" spans="1:7">
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" t="s">
         <v>3</v>
@@ -631,6 +655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -640,7 +665,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -652,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Name: Tan Content:       Add my schedule.
</commit_message>
<xml_diff>
--- a/WeeklySchedule.xlsx
+++ b/WeeklySchedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="C.Thắng" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tân" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Tiết</t>
   </si>
@@ -54,8 +54,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,7 +73,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +116,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -129,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -153,6 +165,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,7 +256,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -277,7 +290,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,21 +465,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="7" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="34.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -506,7 +518,7 @@
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -517,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -525,14 +537,14 @@
       <c r="F3" s="1"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -541,7 +553,7 @@
       <c r="E5" s="1"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -551,17 +563,17 @@
       <c r="F6" s="1"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -571,14 +583,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="6">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -587,7 +599,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -596,24 +608,24 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="6">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -623,28 +635,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="6">
         <v>15</v>
       </c>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="6">
         <v>16</v>
       </c>
       <c r="C19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="E23" s="10" t="s">
         <v>1</v>
       </c>
@@ -653,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="E24" t="s">
         <v>10</v>
       </c>
@@ -662,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="F25" s="3"/>
       <c r="G25" t="s">
         <v>4</v>
@@ -675,20 +687,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="33" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -717,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -732,7 +744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -745,7 +757,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -758,7 +770,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -771,7 +783,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -784,7 +796,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -797,7 +809,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -808,7 +820,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -823,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -836,7 +848,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -849,7 +861,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -862,7 +874,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -875,7 +887,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -888,7 +900,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="6"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -899,7 +911,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -914,7 +926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -927,7 +939,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -940,7 +952,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -959,13 +971,311 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="33" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="6"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="6">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="C20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="C21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>